<commit_message>
added implementation for data provider to read testdata from excel
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/excel/testdata.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27504"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7633D89E-E4C7-4A26-B3B8-EC2232F17AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{73E3571E-AAE7-46B9-BFBF-5140F8AE73DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
+    <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>testname</t>
   </si>
@@ -67,19 +68,63 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>ananya111@gmail.com</t>
+  </si>
+  <si>
+    <t>Ananya@123</t>
+  </si>
+  <si>
+    <t>Ananya</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>trisha@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>trisha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,17 +153,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -517,4 +566,133 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17C0E1D-04E4-4336-A7CD-74BA11CE5F38}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{BE901CD9-8555-4750-B59A-464430492449}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{E1615388-201B-41F7-BE6D-6B19B5A886D2}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{9A8019A2-04AF-476A-A5A6-D0E562866CAF}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{72942F29-E719-4C7D-B150-6FAB49CD3018}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{1500F763-5935-4606-8F16-546D7C7D3493}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented cross browser testing
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27504"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24540FDB-7792-4081-98BD-3B2311868D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8F81BC6-E198-4830-9FE2-AED077C17C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>testname</t>
   </si>
@@ -70,6 +70,9 @@
     <t>2</t>
   </si>
   <si>
+    <t>browser</t>
+  </si>
+  <si>
     <t>username</t>
   </si>
   <si>
@@ -79,6 +82,9 @@
     <t>fname</t>
   </si>
   <si>
+    <t>firefox</t>
+  </si>
+  <si>
     <t>ananya111@gmail.com</t>
   </si>
   <si>
@@ -91,6 +97,9 @@
     <t>no</t>
   </si>
   <si>
+    <t>chrome</t>
+  </si>
+  <si>
     <t>trisha@gmail.com</t>
   </si>
   <si>
@@ -98,9 +107,6 @@
   </si>
   <si>
     <t>trisha</t>
-  </si>
-  <si>
-    <t>Ananya@123dsvgsdf</t>
   </si>
 </sst>
 </file>
@@ -573,20 +579,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17C0E1D-04E4-4336-A7CD-74BA11CE5F38}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,99 +608,117 @@
       <c r="E1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
         <v>20</v>
       </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="E3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
         <v>20</v>
       </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{BE901CD9-8555-4750-B59A-464430492449}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{E1615388-201B-41F7-BE6D-6B19B5A886D2}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{9A8019A2-04AF-476A-A5A6-D0E562866CAF}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{72942F29-E719-4C7D-B150-6FAB49CD3018}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{1500F763-5935-4606-8F16-546D7C7D3493}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BE901CD9-8555-4750-B59A-464430492449}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{E1615388-201B-41F7-BE6D-6B19B5A886D2}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{9A8019A2-04AF-476A-A5A6-D0E562866CAF}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{72942F29-E719-4C7D-B150-6FAB49CD3018}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{1500F763-5935-4606-8F16-546D7C7D3493}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Testscases created for amazon
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27504"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8F81BC6-E198-4830-9FE2-AED077C17C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AC7A044-7722-4E72-A82F-78A9B01A92E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
   <si>
     <t>testname</t>
   </si>
@@ -55,21 +55,30 @@
     <t>To check whether the user can successfully login and logout</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>newtest</t>
+  </si>
+  <si>
+    <t>To check wheather test is executed</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>amazonTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to check the amazon hamburger menu </t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>newtest</t>
-  </si>
-  <si>
-    <t>To check wheather test is executed</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>browser</t>
   </si>
   <si>
@@ -82,6 +91,9 @@
     <t>fname</t>
   </si>
   <si>
+    <t>menutext</t>
+  </si>
+  <si>
     <t>firefox</t>
   </si>
   <si>
@@ -94,7 +106,7 @@
     <t>Ananya</t>
   </si>
   <si>
-    <t>no</t>
+    <t/>
   </si>
   <si>
     <t>chrome</t>
@@ -107,6 +119,9 @@
   </si>
   <si>
     <t>trisha</t>
+  </si>
+  <si>
+    <t>Tablets</t>
   </si>
 </sst>
 </file>
@@ -509,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -572,6 +587,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -579,10 +611,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17C0E1D-04E4-4336-A7CD-74BA11CE5F38}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -590,9 +622,10 @@
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="30.140625" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,19 +633,22 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -620,79 +656,91 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -700,16 +748,42 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>